<commit_message>
Change Address Name to Rep ID  - get rid of custom order and user fields
</commit_message>
<xml_diff>
--- a/app/lib/AddressUploadTemplate.xlsx
+++ b/app/lib/AddressUploadTemplate.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Address Name</t>
+    <t>Rep ID</t>
   </si>
   <si>
     <t>First Name</t>
@@ -47,10 +47,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
     </font>
     <font>
       <b/>
@@ -86,9 +90,12 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -115,31 +122,31 @@
       <c t="s" s="1" r="A1">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c t="s" s="2" r="B1">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c t="s" s="2" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c t="s" s="2" r="D1">
         <v>3</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c t="s" s="2" r="E1">
         <v>4</v>
       </c>
-      <c t="s" s="1" r="F1">
+      <c t="s" s="2" r="F1">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="G1">
+      <c t="s" s="2" r="G1">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="H1">
+      <c t="s" s="2" r="H1">
         <v>7</v>
       </c>
-      <c t="s" s="1" r="I1">
+      <c t="s" s="2" r="I1">
         <v>8</v>
       </c>
-      <c t="s" s="1" r="J1">
+      <c t="s" s="2" r="J1">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PW-12266 - Change Rep ID back to Address Name
</commit_message>
<xml_diff>
--- a/app/lib/AddressUploadTemplate.xlsx
+++ b/app/lib/AddressUploadTemplate.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Rep ID</t>
+    <t>Address Name</t>
   </si>
   <si>
     <t>First Name</t>
@@ -47,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
@@ -60,6 +60,7 @@
       <b/>
       <sz val="11.0"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -90,13 +91,16 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
       <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
+      <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -117,6 +121,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" customWidth="1" max="1" width="15.43"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
@@ -150,6 +157,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2">
+      <c s="3" r="A2"/>
+      <c s="3" r="B2"/>
+      <c s="3" r="C2"/>
+      <c s="3" r="D2"/>
+      <c s="3" r="E2"/>
+      <c s="3" r="G2"/>
+      <c s="3" r="H2"/>
+      <c s="3" r="I2"/>
+      <c s="3" r="J2"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>